<commit_message>
Messy and has some hardcoding but almost done
</commit_message>
<xml_diff>
--- a/Shopify/OrderFromExcel/API/OrderFromThisExcelFile.xlsx
+++ b/Shopify/OrderFromExcel/API/OrderFromThisExcelFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>email</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>Jubilant Jelly</t>
+  </si>
+  <si>
+    <t>Jubilant Jam</t>
+  </si>
+  <si>
+    <t>Peanut Butter</t>
+  </si>
+  <si>
+    <t>Almond Butter</t>
+  </si>
+  <si>
+    <t>Jelly Fish Sandwich</t>
   </si>
 </sst>
 </file>
@@ -405,15 +417,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA64F2A3-17EC-47A9-B25C-93EB76D3746F}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="4" max="4" width="11.64453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -429,20 +444,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
-        <v>6797069778989</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
-        <v>6862783905837</v>
+      <c r="D3">
+        <v>6797069778989</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
         <v>2</v>
+      </c>
+      <c r="D4">
+        <v>6862783905837</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1573432655890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funtional except it double orders
</commit_message>
<xml_diff>
--- a/Shopify/OrderFromExcel/API/OrderFromThisExcelFile.xlsx
+++ b/Shopify/OrderFromExcel/API/OrderFromThisExcelFile.xlsx
@@ -29,9 +29,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>danielvisca96@gmail.com</t>
-  </si>
-  <si>
     <t>shop</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>Jelly Fish Sandwich</t>
+  </si>
+  <si>
+    <t>bubu@send22u.info</t>
   </si>
 </sst>
 </file>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA64F2A3-17EC-47A9-B25C-93EB76D3746F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -428,61 +428,52 @@
     <col min="4" max="4" width="11.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>6797069778989</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>6862783905837</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1573432655890</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Everything is in working order. Tests are partially completed
</commit_message>
<xml_diff>
--- a/Shopify/OrderFromExcel/API/OrderFromThisExcelFile.xlsx
+++ b/Shopify/OrderFromExcel/API/OrderFromThisExcelFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -35,19 +35,31 @@
     <t>Jubilant Jelly</t>
   </si>
   <si>
+    <t>Almond Butter</t>
+  </si>
+  <si>
     <t>Jubilant Jam</t>
   </si>
   <si>
     <t>Peanut Butter</t>
   </si>
   <si>
-    <t>Almond Butter</t>
+    <t>danielvisca96@gmail.com</t>
+  </si>
+  <si>
+    <t>Alan Watts</t>
+  </si>
+  <si>
+    <t>Crepe</t>
   </si>
   <si>
     <t>Jelly Fish Sandwich</t>
   </si>
   <si>
-    <t>bubu@send22u.info</t>
+    <t>The Answer to Life, The Universe and Everything</t>
+  </si>
+  <si>
+    <t>Unjammer</t>
   </si>
 </sst>
 </file>
@@ -71,10 +83,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="4"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -417,14 +430,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA64F2A3-17EC-47A9-B25C-93EB76D3746F}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
+    <col min="1" max="1" width="39.8203125" customWidth="1"/>
+    <col min="2" max="2" width="23.9375" customWidth="1"/>
     <col min="4" max="4" width="11.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -433,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
@@ -446,7 +461,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -454,26 +469,58 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>500</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>